<commit_message>
Update GlobalConfig Add 新增部分逻辑
</commit_message>
<xml_diff>
--- a/target/config.xlsx
+++ b/target/config.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="globalConfig" sheetId="2" r:id="rId1"/>
     <sheet name="sqlConfig" sheetId="1" r:id="rId2"/>
-    <sheet name="Reflection" sheetId="3" r:id="rId3"/>
+    <sheet name="reflection" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>configExplain</t>
   </si>
@@ -40,16 +40,7 @@
     <t>value</t>
   </si>
   <si>
-    <t>是否预组装sql</t>
-  </si>
-  <si>
-    <t>needPreassembly</t>
-  </si>
-  <si>
-    <t>是否需要读sql配置</t>
-  </si>
-  <si>
-    <t>needLoadSqlConfig</t>
+    <t>默认值</t>
   </si>
   <si>
     <t>sql</t>
@@ -59,6 +50,132 @@
 </t>
   </si>
   <si>
+    <t>是否需要读sql配置</t>
+  </si>
+  <si>
+    <t>needLoadSqlConfig</t>
+  </si>
+  <si>
+    <t>sql配置文件的位置</t>
+  </si>
+  <si>
+    <t>sqlConfigPath</t>
+  </si>
+  <si>
+    <t>默认读当前文件sqlConfig Sheet页</t>
+  </si>
+  <si>
+    <t>sql配置文件的sheet页面</t>
+  </si>
+  <si>
+    <t>sqlConfigSheet</t>
+  </si>
+  <si>
+    <t>是否预组装sql</t>
+  </si>
+  <si>
+    <t>needPreassembly</t>
+  </si>
+  <si>
+    <t>是否要读取数据</t>
+  </si>
+  <si>
+    <t>needLoadData</t>
+  </si>
+  <si>
+    <t>方便后续扩展预留字段</t>
+  </si>
+  <si>
+    <t>数据文件存放的位置</t>
+  </si>
+  <si>
+    <t>dataFilePath</t>
+  </si>
+  <si>
+    <t>数据文件sheet页名字</t>
+  </si>
+  <si>
+    <t>dataFileSheet</t>
+  </si>
+  <si>
+    <t>如果有多个sheet直接再写一行</t>
+  </si>
+  <si>
+    <t>是否需要字段映射</t>
+  </si>
+  <si>
+    <t>needFieldsReflection</t>
+  </si>
+  <si>
+    <t>字段映射配置的文件位置</t>
+  </si>
+  <si>
+    <t>fieldsReflectionPath</t>
+  </si>
+  <si>
+    <t>字段映射配置的sheet页面</t>
+  </si>
+  <si>
+    <t>fieldsReflectionSheet</t>
+  </si>
+  <si>
+    <t>是否有需要计算的字段</t>
+  </si>
+  <si>
+    <t>needCalculatedField</t>
+  </si>
+  <si>
+    <t>字段计算类位置</t>
+  </si>
+  <si>
+    <t>calculatedClassPath</t>
+  </si>
+  <si>
+    <t>结果存放的位置</t>
+  </si>
+  <si>
+    <t>resultFilePath</t>
+  </si>
+  <si>
+    <t>默认为jar包所在文件夹下的 resultFile.sql</t>
+  </si>
+  <si>
+    <t>是否保存日志</t>
+  </si>
+  <si>
+    <t>saveLogs</t>
+  </si>
+  <si>
+    <t>日志存放位置</t>
+  </si>
+  <si>
+    <t>logsFilePath</t>
+  </si>
+  <si>
+    <t>默认为jar包所在文件夹下的 logs.txt</t>
+  </si>
+  <si>
+    <t>是否直接保存到数据库</t>
+  </si>
+  <si>
+    <t>saveToDataBase</t>
+  </si>
+  <si>
+    <t>预留字段</t>
+  </si>
+  <si>
+    <t>数据库类型</t>
+  </si>
+  <si>
+    <t>数据库地址/端口</t>
+  </si>
+  <si>
+    <t>账号</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
     <t>SQLType</t>
   </si>
   <si>
@@ -87,6 +204,15 @@
   </si>
   <si>
     <t>tel</t>
+  </si>
+  <si>
+    <t>表中字段名</t>
+  </si>
+  <si>
+    <t>数据库中字段名</t>
+  </si>
+  <si>
+    <t>BT</t>
   </si>
 </sst>
 </file>
@@ -252,12 +378,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -578,7 +716,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -602,16 +740,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -620,90 +758,99 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -712,8 +859,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1240,61 +1399,252 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H20" sqref="H20:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
-    <col min="2" max="2" width="19.375" customWidth="1"/>
-    <col min="3" max="3" width="40.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="2" max="2" width="23.75" customWidth="1"/>
+    <col min="3" max="3" width="40.625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" ht="162" spans="1:3">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="b">
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="b">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:5">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="3" customFormat="1" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" ht="162" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
+      <c r="D19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1309,7 +1659,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1321,40 +1671,40 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="3:5">
       <c r="C4" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1369,14 +1719,35 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>